<commit_message>
messing with hdpi scaling
</commit_message>
<xml_diff>
--- a/Python/server commands.xlsx
+++ b/Python/server commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61e783b3884bd71f/Documents/3_DesignTeams/masa/gui/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84AA8932-399D-4556-B244-FDD976930B7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{84AA8932-399D-4556-B244-FDD976930B7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{77FB1A44-D557-4CE5-8B5E-A294FE6144C4}"/>
   <bookViews>
-    <workbookView xWindow="-21710" yWindow="-4390" windowWidth="21820" windowHeight="38020" xr2:uid="{82AA3AD3-38A4-45D1-BEEF-C48616F86283}"/>
+    <workbookView minimized="1" xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11355" xr2:uid="{82AA3AD3-38A4-45D1-BEEF-C48616F86283}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
     <t>give up command authority</t>
   </si>
   <si>
-    <t>send command to ec</t>
+    <t>send command to board</t>
   </si>
 </sst>
 </file>
@@ -432,18 +432,18 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -474,7 +474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -488,7 +488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -502,7 +502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -519,7 +519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
beta: server packet view table
</commit_message>
<xml_diff>
--- a/Python/server commands.xlsx
+++ b/Python/server commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61e783b3884bd71f/Documents/3_DesignTeams/masa/gui/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{84AA8932-399D-4556-B244-FDD976930B7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{77FB1A44-D557-4CE5-8B5E-A294FE6144C4}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{84AA8932-399D-4556-B244-FDD976930B7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{67D5037A-0B53-4A62-8F3C-7A87741D97E6}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11355" xr2:uid="{82AA3AD3-38A4-45D1-BEEF-C48616F86283}"/>
+    <workbookView xWindow="42720" yWindow="1960" windowWidth="28800" windowHeight="15470" xr2:uid="{82AA3AD3-38A4-45D1-BEEF-C48616F86283}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>command</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>send command to board</t>
+  </si>
+  <si>
+    <t>s2_command() cmd_info</t>
   </si>
 </sst>
 </file>
@@ -432,18 +435,18 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -474,7 +477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -488,7 +491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -502,7 +505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -516,10 +519,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
integrated flash commands with gui and server, ready for testing
</commit_message>
<xml_diff>
--- a/Python/server commands.xlsx
+++ b/Python/server commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61e783b3884bd71f/Documents/3_DesignTeams/masa/gui/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{84AA8932-399D-4556-B244-FDD976930B7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{67D5037A-0B53-4A62-8F3C-7A87741D97E6}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{84AA8932-399D-4556-B244-FDD976930B7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6058F623-5EC7-44E3-8BDF-B9D1E9326DF1}"/>
   <bookViews>
-    <workbookView xWindow="42720" yWindow="1960" windowWidth="28800" windowHeight="15470" xr2:uid="{82AA3AD3-38A4-45D1-BEEF-C48616F86283}"/>
+    <workbookView minimized="1" xWindow="42720" yWindow="1960" windowWidth="28800" windowHeight="15470" xr2:uid="{82AA3AD3-38A4-45D1-BEEF-C48616F86283}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>command</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>s2_command() cmd_info</t>
+  </si>
+  <si>
+    <t>get flash dump</t>
+  </si>
+  <si>
+    <t>target board address</t>
+  </si>
+  <si>
+    <t>dump</t>
   </si>
 </sst>
 </file>
@@ -432,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8554F672-35D6-4802-ABB2-9C19E0EAC1E6}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,6 +545,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added server checkpointing, disabled packet log due to memory issues
</commit_message>
<xml_diff>
--- a/Python/server commands.xlsx
+++ b/Python/server commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61e783b3884bd71f/Documents/3_DesignTeams/masa/gui/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{84AA8932-399D-4556-B244-FDD976930B7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6058F623-5EC7-44E3-8BDF-B9D1E9326DF1}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{84AA8932-399D-4556-B244-FDD976930B7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{96D6D651-9A53-481A-B5EC-AB92070DDA96}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="42720" yWindow="1960" windowWidth="28800" windowHeight="15470" xr2:uid="{82AA3AD3-38A4-45D1-BEEF-C48616F86283}"/>
+    <workbookView xWindow="42720" yWindow="1960" windowWidth="28800" windowHeight="15470" xr2:uid="{82AA3AD3-38A4-45D1-BEEF-C48616F86283}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>command</t>
   </si>
@@ -86,10 +86,19 @@
     <t>get flash dump</t>
   </si>
   <si>
-    <t>target board address</t>
-  </si>
-  <si>
     <t>dump</t>
+  </si>
+  <si>
+    <t>checkpoint</t>
+  </si>
+  <si>
+    <t>creates savefile checkpoint</t>
+  </si>
+  <si>
+    <t>target board address (int)</t>
+  </si>
+  <si>
+    <t>runname (str)</t>
   </si>
 </sst>
 </file>
@@ -441,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8554F672-35D6-4802-ABB2-9C19E0EAC1E6}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,7 +559,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -559,7 +568,24 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
autosequence abort command and input validation
</commit_message>
<xml_diff>
--- a/Python/server commands.xlsx
+++ b/Python/server commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61e783b3884bd71f/Documents/3_DesignTeams/masa/gui/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{84AA8932-399D-4556-B244-FDD976930B7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{96D6D651-9A53-481A-B5EC-AB92070DDA96}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{84AA8932-399D-4556-B244-FDD976930B7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{659F9DDE-7B9C-462C-985A-25562D2215E6}"/>
   <bookViews>
-    <workbookView xWindow="42720" yWindow="1960" windowWidth="28800" windowHeight="15470" xr2:uid="{82AA3AD3-38A4-45D1-BEEF-C48616F86283}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{82AA3AD3-38A4-45D1-BEEF-C48616F86283}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>command</t>
   </si>
@@ -99,6 +99,21 @@
   </si>
   <si>
     <t>runname (str)</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>run autosequence</t>
+  </si>
+  <si>
+    <t>autosequence commands (list)</t>
+  </si>
+  <si>
+    <t>abort_auto</t>
+  </si>
+  <si>
+    <t>abort autosequence</t>
   </si>
 </sst>
 </file>
@@ -450,21 +465,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8554F672-35D6-4802-ABB2-9C19E0EAC1E6}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -495,7 +510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -509,7 +524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -523,7 +538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -540,7 +555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -554,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -571,7 +586,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -586,6 +601,37 @@
       </c>
       <c r="E8" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>